<commit_message>
the import excel finish
</commit_message>
<xml_diff>
--- a/DBCon1/bin/Debug/testread.xlsx
+++ b/DBCon1/bin/Debug/testread.xlsx
@@ -394,7 +394,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -415,7 +415,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>88</v>
+        <v>88.22</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>

</xml_diff>